<commit_message>
Refactor MM, GANTT, PM; delete junk
</commit_message>
<xml_diff>
--- a/PROJECT/GANTT/TINF20C_Gantt_Chart_Team_2_v2.0.xlsx
+++ b/PROJECT/GANTT/TINF20C_Gantt_Chart_Team_2_v2.0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930588FE-6258-4FD1-97C5-5A544533E697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9C2466-B3C0-4E8B-8E1F-E3048C394185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>Erstellen Sie auf diesem Arbeitsblatt einen Projektplan.
 Geben Sie den Titel dieses Projekts in Zelle B1 ein. 
@@ -193,9 +193,6 @@
     <t>Github Aktualisierung</t>
   </si>
   <si>
-    <t>GANTT-Chart 04. Semester</t>
-  </si>
-  <si>
     <t>Prototyping Backend</t>
   </si>
   <si>
@@ -266,6 +263,9 @@
   </si>
   <si>
     <t>Demo Usecase</t>
+  </si>
+  <si>
+    <t>LA</t>
   </si>
 </sst>
 </file>
@@ -1780,11 +1780,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL40"/>
+  <dimension ref="A1:BL39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BS37" sqref="BS37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2497,7 +2497,7 @@
       <c r="F8" s="56"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10" t="str">
-        <f t="shared" ref="H8:H37" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H36" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="28"/>
@@ -2795,7 +2795,7 @@
       <c r="BK11" s="15"/>
       <c r="BL11" s="15"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="18"/>
       <c r="B12" s="50" t="s">
         <v>39</v>
@@ -2874,27 +2874,21 @@
       <c r="BK12" s="15"/>
       <c r="BL12" s="15"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="49">
-        <v>1</v>
-      </c>
-      <c r="E13" s="52">
-        <v>44631</v>
-      </c>
-      <c r="F13" s="52">
-        <v>44645</v>
-      </c>
+    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="62"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="10">
+      <c r="H13" s="10" t="str">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v/>
       </c>
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
@@ -2954,20 +2948,26 @@
       <c r="BL13" s="15"/>
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="61" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="58">
+        <v>1</v>
+      </c>
+      <c r="E14" s="59">
+        <v>44638</v>
+      </c>
+      <c r="F14" s="59">
+        <v>44659</v>
+      </c>
       <c r="G14" s="10"/>
-      <c r="H14" s="10" t="str">
+      <c r="H14" s="10">
         <f t="shared" si="5"/>
-        <v/>
+        <v>22</v>
       </c>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
@@ -2981,8 +2981,8 @@
       <c r="R14" s="28"/>
       <c r="S14" s="28"/>
       <c r="T14" s="28"/>
-      <c r="U14" s="28"/>
-      <c r="V14" s="28"/>
+      <c r="U14" s="29"/>
+      <c r="V14" s="29"/>
       <c r="W14" s="28"/>
       <c r="X14" s="28"/>
       <c r="Y14" s="28"/>
@@ -3026,13 +3026,13 @@
       <c r="BK14" s="15"/>
       <c r="BL14" s="15"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="18"/>
       <c r="B15" s="60" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="57" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" s="58">
         <v>1</v>
@@ -3041,12 +3041,12 @@
         <v>44638</v>
       </c>
       <c r="F15" s="59">
-        <v>44659</v>
+        <v>44661</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I15" s="28"/>
       <c r="J15" s="28"/>
@@ -3060,11 +3060,11 @@
       <c r="R15" s="28"/>
       <c r="S15" s="28"/>
       <c r="T15" s="28"/>
-      <c r="U15" s="29"/>
-      <c r="V15" s="29"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
       <c r="W15" s="28"/>
       <c r="X15" s="28"/>
-      <c r="Y15" s="28"/>
+      <c r="Y15" s="29"/>
       <c r="Z15" s="28"/>
       <c r="AA15" s="28"/>
       <c r="AB15" s="28"/>
@@ -3111,7 +3111,7 @@
         <v>43</v>
       </c>
       <c r="C16" s="57" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D16" s="58">
         <v>1</v>
@@ -3123,10 +3123,7 @@
         <v>44661</v>
       </c>
       <c r="G16" s="10"/>
-      <c r="H16" s="10">
-        <f t="shared" si="5"/>
-        <v>24</v>
-      </c>
+      <c r="H16" s="10"/>
       <c r="I16" s="28"/>
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
@@ -3185,24 +3182,21 @@
       <c r="BL16" s="15"/>
     </row>
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="18"/>
-      <c r="B17" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="58">
-        <v>1</v>
-      </c>
-      <c r="E17" s="59">
-        <v>44638</v>
-      </c>
-      <c r="F17" s="59">
-        <v>44661</v>
-      </c>
+      <c r="A17" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
+      <c r="H17" s="10" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="I17" s="28"/>
       <c r="J17" s="28"/>
       <c r="K17" s="28"/>
@@ -3219,7 +3213,7 @@
       <c r="V17" s="28"/>
       <c r="W17" s="28"/>
       <c r="X17" s="28"/>
-      <c r="Y17" s="29"/>
+      <c r="Y17" s="28"/>
       <c r="Z17" s="28"/>
       <c r="AA17" s="28"/>
       <c r="AB17" s="28"/>
@@ -3260,22 +3254,25 @@
       <c r="BK17" s="15"/>
       <c r="BL17" s="15"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
+    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18"/>
+      <c r="B18" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="34">
+        <v>0.6</v>
+      </c>
+      <c r="E18" s="35">
+        <v>44659</v>
+      </c>
+      <c r="F18" s="35">
+        <v>44673</v>
+      </c>
       <c r="G18" s="10"/>
-      <c r="H18" s="10" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="H18" s="10"/>
       <c r="I18" s="28"/>
       <c r="J18" s="28"/>
       <c r="K18" s="28"/>
@@ -3339,10 +3336,10 @@
         <v>46</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D19" s="34">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E19" s="35">
         <v>44659</v>
@@ -3351,7 +3348,10 @@
         <v>44673</v>
       </c>
       <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="H19" s="10">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
       <c r="I19" s="28"/>
       <c r="J19" s="28"/>
       <c r="K19" s="28"/>
@@ -3415,7 +3415,7 @@
         <v>47</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D20" s="34">
         <v>1</v>
@@ -3431,73 +3431,73 @@
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="28"/>
-      <c r="S20" s="28"/>
-      <c r="T20" s="28"/>
-      <c r="U20" s="28"/>
-      <c r="V20" s="28"/>
-      <c r="W20" s="28"/>
-      <c r="X20" s="28"/>
-      <c r="Y20" s="28"/>
-      <c r="Z20" s="28"/>
-      <c r="AA20" s="28"/>
-      <c r="AB20" s="28"/>
-      <c r="AC20" s="28"/>
-      <c r="AD20" s="28"/>
-      <c r="AE20" s="28"/>
-      <c r="AF20" s="28"/>
-      <c r="AG20" s="28"/>
-      <c r="AH20" s="28"/>
-      <c r="AI20" s="28"/>
-      <c r="AJ20" s="28"/>
-      <c r="AK20" s="28"/>
-      <c r="AL20" s="28"/>
-      <c r="AM20" s="28"/>
-      <c r="AN20" s="28"/>
-      <c r="AO20" s="28"/>
-      <c r="AP20" s="28"/>
-      <c r="AQ20" s="28"/>
-      <c r="AR20" s="28"/>
-      <c r="AS20" s="28"/>
-      <c r="AT20" s="28"/>
-      <c r="AU20" s="28"/>
-      <c r="AV20" s="28"/>
-      <c r="AW20" s="28"/>
-      <c r="AX20" s="28"/>
-      <c r="AY20" s="28"/>
-      <c r="AZ20" s="28"/>
-      <c r="BA20" s="28"/>
-      <c r="BB20" s="28"/>
-      <c r="BC20" s="28"/>
-      <c r="BD20" s="28"/>
-      <c r="BE20" s="28"/>
-      <c r="BF20" s="28"/>
-      <c r="BG20" s="28"/>
-      <c r="BH20" s="28"/>
-      <c r="BI20" s="28"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="15"/>
+      <c r="AB20" s="15"/>
+      <c r="AC20" s="15"/>
+      <c r="AD20" s="15"/>
+      <c r="AE20" s="15"/>
+      <c r="AF20" s="15"/>
+      <c r="AG20" s="15"/>
+      <c r="AH20" s="15"/>
+      <c r="AI20" s="15"/>
+      <c r="AJ20" s="15"/>
+      <c r="AK20" s="15"/>
+      <c r="AL20" s="15"/>
+      <c r="AM20" s="15"/>
+      <c r="AN20" s="15"/>
+      <c r="AO20" s="15"/>
+      <c r="AP20" s="15"/>
+      <c r="AQ20" s="15"/>
+      <c r="AR20" s="15"/>
+      <c r="AS20" s="15"/>
+      <c r="AT20" s="15"/>
+      <c r="AU20" s="15"/>
+      <c r="AV20" s="15"/>
+      <c r="AW20" s="15"/>
+      <c r="AX20" s="15"/>
+      <c r="AY20" s="15"/>
+      <c r="AZ20" s="15"/>
+      <c r="BA20" s="15"/>
+      <c r="BB20" s="15"/>
+      <c r="BC20" s="15"/>
+      <c r="BD20" s="15"/>
+      <c r="BE20" s="15"/>
+      <c r="BF20" s="15"/>
+      <c r="BG20" s="15"/>
+      <c r="BH20" s="15"/>
+      <c r="BI20" s="15"/>
       <c r="BJ20" s="15"/>
       <c r="BK20" s="15"/>
       <c r="BL20" s="15"/>
     </row>
-    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18"/>
       <c r="B21" s="36" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D21" s="34">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E21" s="35">
         <v>44659</v>
@@ -3506,10 +3506,7 @@
         <v>44673</v>
       </c>
       <c r="G21" s="10"/>
-      <c r="H21" s="10">
-        <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
+      <c r="H21" s="10"/>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
@@ -3569,21 +3566,13 @@
     </row>
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18"/>
-      <c r="B22" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="E22" s="35">
-        <v>44659</v>
-      </c>
-      <c r="F22" s="35">
-        <v>44673</v>
-      </c>
+      <c r="B22" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="15"/>
@@ -3643,15 +3632,23 @@
       <c r="BK22" s="15"/>
       <c r="BL22" s="15"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18"/>
-      <c r="B23" s="41" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
+      <c r="B23" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="47">
+        <v>1</v>
+      </c>
+      <c r="E23" s="48">
+        <v>44673</v>
+      </c>
+      <c r="F23" s="48">
+        <v>44682</v>
+      </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
       <c r="I23" s="15"/>
@@ -3717,7 +3714,7 @@
         <v>52</v>
       </c>
       <c r="C24" s="46" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D24" s="47">
         <v>1</v>
@@ -3787,13 +3784,13 @@
       <c r="BK24" s="15"/>
       <c r="BL24" s="15"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="18"/>
-      <c r="B25" s="45" t="s">
-        <v>53</v>
+      <c r="B25" s="76" t="s">
+        <v>60</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="D25" s="47">
         <v>1</v>
@@ -3865,21 +3862,13 @@
     </row>
     <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18"/>
-      <c r="B26" s="76" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="47">
-        <v>1</v>
-      </c>
-      <c r="E26" s="48">
-        <v>44673</v>
-      </c>
-      <c r="F26" s="48">
-        <v>44682</v>
-      </c>
+      <c r="B26" s="71" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="72"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="15"/>
@@ -3941,13 +3930,21 @@
     </row>
     <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="18"/>
-      <c r="B27" s="71" t="s">
+      <c r="B27" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="72"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
+      <c r="C27" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="55">
+        <v>1</v>
+      </c>
+      <c r="E27" s="56">
+        <v>44682</v>
+      </c>
+      <c r="F27" s="56">
+        <v>44687</v>
+      </c>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
       <c r="I27" s="15"/>
@@ -4010,11 +4007,9 @@
     <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="18"/>
       <c r="B28" s="75" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="54" t="s">
-        <v>36</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C28" s="54"/>
       <c r="D28" s="55">
         <v>1</v>
       </c>
@@ -4022,7 +4017,7 @@
         <v>44682</v>
       </c>
       <c r="F28" s="56">
-        <v>44689</v>
+        <v>44687</v>
       </c>
       <c r="G28" s="10"/>
       <c r="H28" s="10"/>
@@ -4086,7 +4081,7 @@
     <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18"/>
       <c r="B29" s="75" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C29" s="54"/>
       <c r="D29" s="55">
@@ -4096,7 +4091,7 @@
         <v>44682</v>
       </c>
       <c r="F29" s="56">
-        <v>44689</v>
+        <v>44687</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="10"/>
@@ -4160,9 +4155,11 @@
     <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18"/>
       <c r="B30" s="75" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="54"/>
+        <v>49</v>
+      </c>
+      <c r="C30" s="54" t="s">
+        <v>31</v>
+      </c>
       <c r="D30" s="55">
         <v>1</v>
       </c>
@@ -4170,7 +4167,7 @@
         <v>44682</v>
       </c>
       <c r="F30" s="56">
-        <v>44689</v>
+        <v>44687</v>
       </c>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
@@ -4234,7 +4231,7 @@
     <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="18"/>
       <c r="B31" s="75" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C31" s="54" t="s">
         <v>31</v>
@@ -4246,7 +4243,7 @@
         <v>44682</v>
       </c>
       <c r="F31" s="56">
-        <v>44689</v>
+        <v>44687</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
@@ -4310,10 +4307,10 @@
     <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18"/>
       <c r="B32" s="75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="54" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D32" s="55">
         <v>1</v>
@@ -4322,7 +4319,7 @@
         <v>44682</v>
       </c>
       <c r="F32" s="56">
-        <v>44694</v>
+        <v>44687</v>
       </c>
       <c r="G32" s="10"/>
       <c r="H32" s="10"/>
@@ -4386,7 +4383,7 @@
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18"/>
       <c r="B33" s="77" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="78"/>
       <c r="D33" s="79"/>
@@ -4454,19 +4451,19 @@
     <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="18"/>
       <c r="B34" s="81" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C34" s="82" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D34" s="83">
         <v>1</v>
       </c>
       <c r="E34" s="84">
-        <v>44689</v>
+        <v>44687</v>
       </c>
       <c r="F34" s="84">
-        <v>44694</v>
+        <v>44693</v>
       </c>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -4530,7 +4527,7 @@
     <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18"/>
       <c r="B35" s="81" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C35" s="82" t="s">
         <v>22</v>
@@ -4539,10 +4536,10 @@
         <v>1</v>
       </c>
       <c r="E35" s="84">
-        <v>44689</v>
+        <v>44687</v>
       </c>
       <c r="F35" s="84">
-        <v>44694</v>
+        <v>44693</v>
       </c>
       <c r="G35" s="10"/>
       <c r="H35" s="10"/>
@@ -4604,163 +4601,87 @@
       <c r="BL35" s="15"/>
     </row>
     <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="18"/>
-      <c r="B36" s="81" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="82" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="83">
-        <v>1</v>
-      </c>
-      <c r="E36" s="84">
-        <v>44689</v>
-      </c>
-      <c r="F36" s="84">
-        <v>44694</v>
-      </c>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="15"/>
-      <c r="U36" s="15"/>
-      <c r="V36" s="15"/>
-      <c r="W36" s="15"/>
-      <c r="X36" s="15"/>
-      <c r="Y36" s="15"/>
-      <c r="Z36" s="15"/>
-      <c r="AA36" s="15"/>
-      <c r="AB36" s="15"/>
-      <c r="AC36" s="15"/>
-      <c r="AD36" s="15"/>
-      <c r="AE36" s="15"/>
-      <c r="AF36" s="15"/>
-      <c r="AG36" s="15"/>
-      <c r="AH36" s="15"/>
-      <c r="AI36" s="15"/>
-      <c r="AJ36" s="15"/>
-      <c r="AK36" s="15"/>
-      <c r="AL36" s="15"/>
-      <c r="AM36" s="15"/>
-      <c r="AN36" s="15"/>
-      <c r="AO36" s="15"/>
-      <c r="AP36" s="15"/>
-      <c r="AQ36" s="15"/>
-      <c r="AR36" s="15"/>
-      <c r="AS36" s="15"/>
-      <c r="AT36" s="15"/>
-      <c r="AU36" s="15"/>
-      <c r="AV36" s="15"/>
-      <c r="AW36" s="15"/>
-      <c r="AX36" s="15"/>
-      <c r="AY36" s="15"/>
-      <c r="AZ36" s="15"/>
-      <c r="BA36" s="15"/>
-      <c r="BB36" s="15"/>
-      <c r="BC36" s="15"/>
-      <c r="BD36" s="15"/>
-      <c r="BE36" s="15"/>
-      <c r="BF36" s="15"/>
-      <c r="BG36" s="15"/>
-      <c r="BH36" s="15"/>
-      <c r="BI36" s="15"/>
-      <c r="BJ36" s="15"/>
-      <c r="BK36" s="15"/>
-      <c r="BL36" s="15"/>
-    </row>
-    <row r="37" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
+      <c r="A36" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B36" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14" t="str">
+      <c r="C36" s="12"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="16"/>
-      <c r="N37" s="16"/>
-      <c r="O37" s="16"/>
-      <c r="P37" s="16"/>
-      <c r="Q37" s="16"/>
-      <c r="R37" s="16"/>
-      <c r="S37" s="16"/>
-      <c r="T37" s="16"/>
-      <c r="U37" s="16"/>
-      <c r="V37" s="16"/>
-      <c r="W37" s="16"/>
-      <c r="X37" s="16"/>
-      <c r="Y37" s="16"/>
-      <c r="Z37" s="16"/>
-      <c r="AA37" s="16"/>
-      <c r="AB37" s="16"/>
-      <c r="AC37" s="16"/>
-      <c r="AD37" s="16"/>
-      <c r="AE37" s="16"/>
-      <c r="AF37" s="16"/>
-      <c r="AG37" s="16"/>
-      <c r="AH37" s="16"/>
-      <c r="AI37" s="16"/>
-      <c r="AJ37" s="16"/>
-      <c r="AK37" s="16"/>
-      <c r="AL37" s="16"/>
-      <c r="AM37" s="16"/>
-      <c r="AN37" s="16"/>
-      <c r="AO37" s="16"/>
-      <c r="AP37" s="16"/>
-      <c r="AQ37" s="16"/>
-      <c r="AR37" s="16"/>
-      <c r="AS37" s="16"/>
-      <c r="AT37" s="16"/>
-      <c r="AU37" s="16"/>
-      <c r="AV37" s="16"/>
-      <c r="AW37" s="16"/>
-      <c r="AX37" s="16"/>
-      <c r="AY37" s="16"/>
-      <c r="AZ37" s="16"/>
-      <c r="BA37" s="16"/>
-      <c r="BB37" s="16"/>
-      <c r="BC37" s="16"/>
-      <c r="BD37" s="16"/>
-      <c r="BE37" s="16"/>
-      <c r="BF37" s="16"/>
-      <c r="BG37" s="16"/>
-      <c r="BH37" s="16"/>
-      <c r="BI37" s="16"/>
-      <c r="BJ37" s="16"/>
-      <c r="BK37" s="16"/>
-      <c r="BL37" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="16"/>
+      <c r="U36" s="16"/>
+      <c r="V36" s="16"/>
+      <c r="W36" s="16"/>
+      <c r="X36" s="16"/>
+      <c r="Y36" s="16"/>
+      <c r="Z36" s="16"/>
+      <c r="AA36" s="16"/>
+      <c r="AB36" s="16"/>
+      <c r="AC36" s="16"/>
+      <c r="AD36" s="16"/>
+      <c r="AE36" s="16"/>
+      <c r="AF36" s="16"/>
+      <c r="AG36" s="16"/>
+      <c r="AH36" s="16"/>
+      <c r="AI36" s="16"/>
+      <c r="AJ36" s="16"/>
+      <c r="AK36" s="16"/>
+      <c r="AL36" s="16"/>
+      <c r="AM36" s="16"/>
+      <c r="AN36" s="16"/>
+      <c r="AO36" s="16"/>
+      <c r="AP36" s="16"/>
+      <c r="AQ36" s="16"/>
+      <c r="AR36" s="16"/>
+      <c r="AS36" s="16"/>
+      <c r="AT36" s="16"/>
+      <c r="AU36" s="16"/>
+      <c r="AV36" s="16"/>
+      <c r="AW36" s="16"/>
+      <c r="AX36" s="16"/>
+      <c r="AY36" s="16"/>
+      <c r="AZ36" s="16"/>
+      <c r="BA36" s="16"/>
+      <c r="BB36" s="16"/>
+      <c r="BC36" s="16"/>
+      <c r="BD36" s="16"/>
+      <c r="BE36" s="16"/>
+      <c r="BF36" s="16"/>
+      <c r="BG36" s="16"/>
+      <c r="BH36" s="16"/>
+      <c r="BI36" s="16"/>
+      <c r="BJ36" s="16"/>
+      <c r="BK36" s="16"/>
+      <c r="BL36" s="16"/>
+    </row>
+    <row r="37" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="6"/>
     </row>
     <row r="38" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G38" s="6"/>
+      <c r="C38" s="8"/>
+      <c r="F38" s="20"/>
     </row>
     <row r="39" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="8"/>
-      <c r="F39" s="20"/>
-    </row>
-    <row r="40" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="9"/>
+      <c r="C39" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -4775,7 +4696,7 @@
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D9:D13 D24:D26">
+  <conditionalFormatting sqref="D9:D12 D23:D25 D34:D35 D31">
     <cfRule type="dataBar" priority="41">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4789,12 +4710,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL37">
+  <conditionalFormatting sqref="I5:BL36">
     <cfRule type="expression" dxfId="2" priority="60">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL37">
+  <conditionalFormatting sqref="I7:BL36">
     <cfRule type="expression" dxfId="1" priority="54">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4802,7 +4723,7 @@
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34:D36 D28:D32">
+  <conditionalFormatting sqref="D27:D32">
     <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4816,7 +4737,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
+  <conditionalFormatting sqref="D18">
     <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4830,7 +4751,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
+  <conditionalFormatting sqref="D14">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4844,7 +4765,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
+  <conditionalFormatting sqref="D15">
     <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4858,7 +4779,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
+  <conditionalFormatting sqref="D16">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4872,7 +4793,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
+  <conditionalFormatting sqref="D19">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4886,7 +4807,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
+  <conditionalFormatting sqref="D20">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4900,7 +4821,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
+  <conditionalFormatting sqref="D21">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4914,7 +4835,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D30:D31">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4955,7 +4876,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D9:D13 D24:D26</xm:sqref>
+          <xm:sqref>D9:D12 D23:D25 D34:D35 D31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{76AAB79F-4ACA-4D58-8097-95BC0DA9DDE2}">
@@ -4970,7 +4891,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D34:D36 D28:D32</xm:sqref>
+          <xm:sqref>D27:D32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{06D96D9C-7FBF-476C-A1C2-4BDCD80B21E2}">
@@ -4985,7 +4906,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D19</xm:sqref>
+          <xm:sqref>D18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{2A54C957-F6D4-4BC6-B4E4-137857B2EB02}">
@@ -5000,7 +4921,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D15</xm:sqref>
+          <xm:sqref>D14</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{AE11CDF7-BC23-4756-AE31-E8109B308750}">
@@ -5015,7 +4936,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D16</xm:sqref>
+          <xm:sqref>D15</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{ED084AAE-862D-4E8F-B052-47E548E0CEA0}">
@@ -5030,7 +4951,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D17</xm:sqref>
+          <xm:sqref>D16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F065563F-BEF3-4FAB-9BDD-946EFFCF42EE}">
@@ -5045,7 +4966,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D20</xm:sqref>
+          <xm:sqref>D19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4CC3855D-C738-4FBD-B24B-3479663A244A}">
@@ -5060,7 +4981,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D21</xm:sqref>
+          <xm:sqref>D20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{9867D7E9-6EDE-4315-805C-1CDE0AD3AB70}">
@@ -5075,7 +4996,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D22</xm:sqref>
+          <xm:sqref>D21</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{425AB7CC-B32C-4295-8191-D4ADC2FE2881}">
@@ -5090,7 +5011,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D31</xm:sqref>
+          <xm:sqref>D30:D31</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>